<commit_message>
20250929_commit this is working code . about to refactor to change et array to etr average.
</commit_message>
<xml_diff>
--- a/combined_cal_data.xlsx
+++ b/combined_cal_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINER\Documents\PycharmProjects\20250804_Power_Servo\src\measurements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINER\Documents\PycharmProjects\20250926_EVM_DPD_DDPD_GMP_Power_Servo_with_test_select\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A4763-D5F1-4269-B29C-E57FBDBAF1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF1029-909E-4968-8475-D3A4A146C8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27888" yWindow="2148" windowWidth="27000" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25848" yWindow="1044" windowWidth="25632" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Calibration" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -463,7 +463,7 @@
         <v>15.819000000000001</v>
       </c>
       <c r="E2">
-        <v>1.5880000000000001</v>
+        <v>1.6384837962300001</v>
       </c>
       <c r="F2">
         <v>10.186999999999999</v>
@@ -483,7 +483,7 @@
         <v>15.942</v>
       </c>
       <c r="E3">
-        <v>1.603</v>
+        <v>1.6586218803099999</v>
       </c>
       <c r="F3">
         <v>10.311999999999999</v>
@@ -503,7 +503,7 @@
         <v>16.05</v>
       </c>
       <c r="E4">
-        <v>1.615</v>
+        <v>1.69783757327</v>
       </c>
       <c r="F4">
         <v>10.519</v>
@@ -523,7 +523,7 @@
         <v>16.123999999999999</v>
       </c>
       <c r="E5">
-        <v>1.583</v>
+        <v>1.66663520516</v>
       </c>
       <c r="F5">
         <v>10.755000000000001</v>
@@ -543,7 +543,7 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E6">
-        <v>1.577</v>
+        <v>1.6394822981399999</v>
       </c>
       <c r="F6">
         <v>11.042</v>
@@ -563,7 +563,7 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E7">
-        <v>1.58</v>
+        <v>1.6707124931300001</v>
       </c>
       <c r="F7">
         <v>11.314</v>
@@ -583,7 +583,7 @@
         <v>16.125</v>
       </c>
       <c r="E8">
-        <v>1.5289999999999999</v>
+        <v>1.5562517593499998</v>
       </c>
       <c r="F8">
         <v>11.442</v>
@@ -603,7 +603,7 @@
         <v>16.055</v>
       </c>
       <c r="E9">
-        <v>1.605</v>
+        <v>1.6695577590899999</v>
       </c>
       <c r="F9">
         <v>11.582000000000001</v>
@@ -623,7 +623,7 @@
         <v>15.952</v>
       </c>
       <c r="E10">
-        <v>1.6160000000000001</v>
+        <v>1.6901819344600002</v>
       </c>
       <c r="F10">
         <v>11.516</v>
@@ -643,7 +643,7 @@
         <v>15.826000000000001</v>
       </c>
       <c r="E11">
-        <v>1.5820000000000001</v>
+        <v>1.6327185529300001</v>
       </c>
       <c r="F11">
         <v>11.281000000000001</v>
@@ -663,7 +663,7 @@
         <v>15.7</v>
       </c>
       <c r="E12">
-        <v>1.669</v>
+        <v>1.6529666815700002</v>
       </c>
       <c r="F12">
         <v>11.09</v>
@@ -683,7 +683,7 @@
         <v>15.579000000000001</v>
       </c>
       <c r="E13">
-        <v>1.6759999999999999</v>
+        <v>1.6806430130099999</v>
       </c>
       <c r="F13">
         <v>10.792999999999999</v>
@@ -703,7 +703,7 @@
         <v>15.467000000000001</v>
       </c>
       <c r="E14">
-        <v>1.6839999999999999</v>
+        <v>1.7207988732899999</v>
       </c>
       <c r="F14">
         <v>10.523</v>
@@ -723,7 +723,7 @@
         <v>15.382999999999999</v>
       </c>
       <c r="E15">
-        <v>1.748</v>
+        <v>1.7680798639299999</v>
       </c>
       <c r="F15">
         <v>10.372999999999999</v>
@@ -743,7 +743,7 @@
         <v>15.326000000000001</v>
       </c>
       <c r="E16">
-        <v>1.7569999999999999</v>
+        <v>1.8414640190599998</v>
       </c>
       <c r="F16">
         <v>10.257999999999999</v>
@@ -763,7 +763,7 @@
         <v>15.297000000000001</v>
       </c>
       <c r="E17">
-        <v>1.7949999999999999</v>
+        <v>1.84070112484</v>
       </c>
       <c r="F17">
         <v>10.271000000000001</v>
@@ -783,7 +783,7 @@
         <v>15.305999999999999</v>
       </c>
       <c r="E18">
-        <v>1.8</v>
+        <v>1.8190075346300001</v>
       </c>
       <c r="F18">
         <v>10.359</v>
@@ -803,7 +803,7 @@
         <v>15.345000000000001</v>
       </c>
       <c r="E19">
-        <v>1.7689999999999999</v>
+        <v>1.78324713921</v>
       </c>
       <c r="F19">
         <v>10.502000000000001</v>
@@ -823,7 +823,7 @@
         <v>15.414999999999999</v>
       </c>
       <c r="E20">
-        <v>1.784</v>
+        <v>1.8669747491299999</v>
       </c>
       <c r="F20">
         <v>10.763</v>
@@ -843,7 +843,7 @@
         <v>15.513999999999999</v>
       </c>
       <c r="E21">
-        <v>1.806</v>
+        <v>1.8833715236700002</v>
       </c>
       <c r="F21">
         <v>11.071</v>
@@ -863,7 +863,7 @@
         <v>15.627000000000001</v>
       </c>
       <c r="E22">
-        <v>1.7350000000000001</v>
+        <v>1.7462585513500002</v>
       </c>
       <c r="F22">
         <v>11.282</v>
@@ -883,7 +883,7 @@
         <v>15.756</v>
       </c>
       <c r="E23">
-        <v>1.7949999999999999</v>
+        <v>1.8775014061699999</v>
       </c>
       <c r="F23">
         <v>11.567</v>
@@ -903,7 +903,7 @@
         <v>15.888</v>
       </c>
       <c r="E24">
-        <v>1.837</v>
+        <v>1.8444125277249999</v>
       </c>
       <c r="F24">
         <v>11.724</v>
@@ -923,7 +923,7 @@
         <v>16.010000000000002</v>
       </c>
       <c r="E25">
-        <v>1.8380000000000001</v>
+        <v>1.82673410661</v>
       </c>
       <c r="F25">
         <v>11.706</v>
@@ -943,7 +943,7 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E26">
-        <v>1.85</v>
+        <v>1.9237036086000001</v>
       </c>
       <c r="F26">
         <v>11.564</v>
@@ -963,7 +963,7 @@
         <v>16.183</v>
       </c>
       <c r="E27">
-        <v>1.87</v>
+        <v>1.8607387499650001</v>
       </c>
       <c r="F27">
         <v>11.334</v>
@@ -983,7 +983,7 @@
         <v>16.216000000000001</v>
       </c>
       <c r="E28">
-        <v>1.9039999999999999</v>
+        <v>1.83742717552</v>
       </c>
       <c r="F28">
         <v>11.068</v>
@@ -1003,7 +1003,7 @@
         <v>16.209</v>
       </c>
       <c r="E29">
-        <v>1.9339999999999999</v>
+        <v>1.96477983914</v>
       </c>
       <c r="F29">
         <v>10.801</v>
@@ -1023,7 +1023,7 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E30">
-        <v>1.966</v>
+        <v>1.9203338963600001</v>
       </c>
       <c r="F30">
         <v>10.59</v>
@@ -1043,7 +1043,7 @@
         <v>16.091999999999999</v>
       </c>
       <c r="E31">
-        <v>1.978</v>
+        <v>1.9600063868099999</v>
       </c>
       <c r="F31">
         <v>10.442</v>
@@ -1063,7 +1063,7 @@
         <v>15.987</v>
       </c>
       <c r="E32">
-        <v>2.012</v>
+        <v>2.1004507234199998</v>
       </c>
       <c r="F32">
         <v>10.411</v>
@@ -1083,7 +1083,7 @@
         <v>15.872</v>
       </c>
       <c r="E33">
-        <v>2.04</v>
+        <v>2.0897662510199999</v>
       </c>
       <c r="F33">
         <v>10.468</v>
@@ -1103,7 +1103,7 @@
         <v>15.749000000000001</v>
       </c>
       <c r="E34">
-        <v>2.008</v>
+        <v>1.9686865043699999</v>
       </c>
       <c r="F34">
         <v>10.561</v>
@@ -1123,7 +1123,7 @@
         <v>15.634</v>
       </c>
       <c r="E35">
-        <v>2.02</v>
+        <v>1.98511326897</v>
       </c>
       <c r="F35">
         <v>10.781000000000001</v>
@@ -1143,7 +1143,7 @@
         <v>15.532</v>
       </c>
       <c r="E36">
-        <v>2.0310000000000001</v>
+        <v>2.0487600563999999</v>
       </c>
       <c r="F36">
         <v>11.047000000000001</v>
@@ -1163,7 +1163,7 @@
         <v>15.46</v>
       </c>
       <c r="E37">
-        <v>1.986</v>
+        <v>2.0188485269599998</v>
       </c>
       <c r="F37">
         <v>11.278</v>
@@ -1183,7 +1183,7 @@
         <v>15.414</v>
       </c>
       <c r="E38">
-        <v>2.0030000000000001</v>
+        <v>2.0895582085600002</v>
       </c>
       <c r="F38">
         <v>11.53</v>
@@ -1203,7 +1203,7 @@
         <v>15.393000000000001</v>
       </c>
       <c r="E39">
-        <v>1.992</v>
+        <v>2.1455872832999998</v>
       </c>
       <c r="F39">
         <v>11.672000000000001</v>
@@ -1223,7 +1223,7 @@
         <v>15.407999999999999</v>
       </c>
       <c r="E40">
-        <v>1.992</v>
+        <v>2.0128021831899998</v>
       </c>
       <c r="F40">
         <v>11.712</v>
@@ -1243,7 +1243,7 @@
         <v>15.451000000000001</v>
       </c>
       <c r="E41">
-        <v>2.0299999999999998</v>
+        <v>1.9354800532399998</v>
       </c>
       <c r="F41">
         <v>11.635</v>
@@ -1263,7 +1263,7 @@
         <v>15.521000000000001</v>
       </c>
       <c r="E42">
-        <v>2.0579999999999998</v>
+        <v>2.01036161066</v>
       </c>
       <c r="F42">
         <v>11.459</v>
@@ -1283,7 +1283,7 @@
         <v>15.61</v>
       </c>
       <c r="E43">
-        <v>2.0739999999999998</v>
+        <v>2.1985707115999999</v>
       </c>
       <c r="F43">
         <v>11.201000000000001</v>
@@ -1303,7 +1303,7 @@
         <v>15.718</v>
       </c>
       <c r="E44">
-        <v>2.0910000000000002</v>
+        <v>2.0687919849500003</v>
       </c>
       <c r="F44">
         <v>10.929</v>
@@ -1323,7 +1323,7 @@
         <v>15.831</v>
       </c>
       <c r="E45">
-        <v>2.1989999999999998</v>
+        <v>2.1388264352799999</v>
       </c>
       <c r="F45">
         <v>10.804</v>
@@ -1343,7 +1343,7 @@
         <v>15.949</v>
       </c>
       <c r="E46">
-        <v>2.1989999999999998</v>
+        <v>2.19407232391</v>
       </c>
       <c r="F46">
         <v>10.603</v>
@@ -1363,7 +1363,7 @@
         <v>16.058</v>
       </c>
       <c r="E47">
-        <v>2.1659999999999999</v>
+        <v>2.1778569245499999</v>
       </c>
       <c r="F47">
         <v>10.468</v>
@@ -1383,7 +1383,7 @@
         <v>16.151</v>
       </c>
       <c r="E48">
-        <v>2.2570000000000001</v>
+        <v>2.2173617492000002</v>
       </c>
       <c r="F48">
         <v>10.532999999999999</v>
@@ -1403,7 +1403,7 @@
         <v>16.212</v>
       </c>
       <c r="E49">
-        <v>2.2149999999999999</v>
+        <v>2.2300445945599998</v>
       </c>
       <c r="F49">
         <v>10.544</v>
@@ -1423,7 +1423,7 @@
         <v>16.238</v>
       </c>
       <c r="E50">
-        <v>2.198</v>
+        <v>2.1968254528358999</v>
       </c>
       <c r="F50">
         <v>10.670999999999999</v>
@@ -1443,7 +1443,7 @@
         <v>16.225999999999999</v>
       </c>
       <c r="E51">
-        <v>2.2000000000000002</v>
+        <v>2.24478663353</v>
       </c>
       <c r="F51">
         <v>10.882999999999999</v>
@@ -1463,7 +1463,7 @@
         <v>16.184000000000001</v>
       </c>
       <c r="E52">
-        <v>2.2050000000000001</v>
+        <v>2.2341556567500001</v>
       </c>
       <c r="F52">
         <v>11.115</v>
@@ -1483,7 +1483,7 @@
         <v>16.106000000000002</v>
       </c>
       <c r="E53">
-        <v>2.2029999999999998</v>
+        <v>2.2113324208139997</v>
       </c>
       <c r="F53">
         <v>11.343999999999999</v>
@@ -1503,7 +1503,7 @@
         <v>16.007999999999999</v>
       </c>
       <c r="E54">
-        <v>2.1739999999999999</v>
+        <v>2.1556990335499999</v>
       </c>
       <c r="F54">
         <v>11.472</v>
@@ -1523,7 +1523,7 @@
         <v>15.896000000000001</v>
       </c>
       <c r="E55">
-        <v>2.1890000000000001</v>
+        <v>2.2393885515200003</v>
       </c>
       <c r="F55">
         <v>11.555</v>
@@ -1543,7 +1543,7 @@
         <v>15.784000000000001</v>
       </c>
       <c r="E56">
-        <v>2.1779999999999999</v>
+        <v>2.2712320039099998</v>
       </c>
       <c r="F56">
         <v>11.504</v>
@@ -1563,7 +1563,7 @@
         <v>15.682</v>
       </c>
       <c r="E57">
-        <v>2.2909999999999999</v>
+        <v>2.2958746626240001</v>
       </c>
       <c r="F57">
         <v>11.465999999999999</v>
@@ -1583,7 +1583,7 @@
         <v>15.587</v>
       </c>
       <c r="E58">
-        <v>2.2240000000000002</v>
+        <v>2.2380031172500003</v>
       </c>
       <c r="F58">
         <v>11.195</v>
@@ -1603,7 +1603,7 @@
         <v>15.512</v>
       </c>
       <c r="E59">
-        <v>2.2069999999999999</v>
+        <v>2.1561174938400001</v>
       </c>
       <c r="F59">
         <v>10.919</v>
@@ -1623,7 +1623,7 @@
         <v>15.46</v>
       </c>
       <c r="E60">
-        <v>2.343</v>
+        <v>2.3908738164700001</v>
       </c>
       <c r="F60">
         <v>10.821999999999999</v>
@@ -1643,7 +1643,7 @@
         <v>15.423999999999999</v>
       </c>
       <c r="E61">
-        <v>2.3519999999999999</v>
+        <v>2.3444008994765997</v>
       </c>
       <c r="F61">
         <v>10.624000000000001</v>
@@ -1663,7 +1663,7 @@
         <v>15.425000000000001</v>
       </c>
       <c r="E62">
-        <v>2.37</v>
+        <v>2.32682532251</v>
       </c>
       <c r="F62">
         <v>10.513</v>
@@ -1683,7 +1683,7 @@
         <v>15.445</v>
       </c>
       <c r="E63">
-        <v>2.415</v>
+        <v>2.4198693923870001</v>
       </c>
       <c r="F63">
         <v>10.505000000000001</v>
@@ -1703,7 +1703,7 @@
         <v>15.497</v>
       </c>
       <c r="E64">
-        <v>2.4409999999999998</v>
+        <v>2.7707788727999998</v>
       </c>
       <c r="F64">
         <v>10.573</v>
@@ -1723,7 +1723,7 @@
         <v>15.574999999999999</v>
       </c>
       <c r="E65">
-        <v>2.4319999999999999</v>
+        <v>2.6148606409999999</v>
       </c>
       <c r="F65">
         <v>10.68</v>
@@ -1743,7 +1743,7 @@
         <v>15.673</v>
       </c>
       <c r="E66">
-        <v>2.4319999999999999</v>
+        <v>2.5843345257000001</v>
       </c>
       <c r="F66">
         <v>10.881</v>
@@ -1763,7 +1763,7 @@
         <v>15.789</v>
       </c>
       <c r="E67">
-        <v>2.4129999999999998</v>
+        <v>2.5671409818999997</v>
       </c>
       <c r="F67">
         <v>11.102</v>
@@ -1783,7 +1783,7 @@
         <v>15.901</v>
       </c>
       <c r="E68">
-        <v>2.3620000000000001</v>
+        <v>2.4475936934</v>
       </c>
       <c r="F68">
         <v>11.29</v>
@@ -1803,7 +1803,7 @@
         <v>16.012</v>
       </c>
       <c r="E69">
-        <v>2.4129999999999998</v>
+        <v>2.5853386400999998</v>
       </c>
       <c r="F69">
         <v>11.574</v>
@@ -1823,7 +1823,7 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E70">
-        <v>2.4129999999999998</v>
+        <v>2.5519596187999998</v>
       </c>
       <c r="F70">
         <v>11.696999999999999</v>
@@ -1843,7 +1843,7 @@
         <v>16.184999999999999</v>
       </c>
       <c r="E71">
-        <v>2.387</v>
+        <v>2.5514894947000002</v>
       </c>
       <c r="F71">
         <v>11.728999999999999</v>
@@ -1863,7 +1863,7 @@
         <v>16.224</v>
       </c>
       <c r="E72">
-        <v>2.411</v>
+        <v>2.5813201328000002</v>
       </c>
       <c r="F72">
         <v>11.672000000000001</v>
@@ -1883,7 +1883,7 @@
         <v>16.239000000000001</v>
       </c>
       <c r="E73">
-        <v>2.4740000000000002</v>
+        <v>2.6591293584000004</v>
       </c>
       <c r="F73">
         <v>11.566000000000001</v>
@@ -1903,7 +1903,7 @@
         <v>16.222000000000001</v>
       </c>
       <c r="E74">
-        <v>2.484</v>
+        <v>2.6963444582</v>
       </c>
       <c r="F74">
         <v>11.347</v>
@@ -1923,7 +1923,7 @@
         <v>16.175999999999998</v>
       </c>
       <c r="E75">
-        <v>2.4769999999999999</v>
+        <v>2.5840228168999997</v>
       </c>
       <c r="F75">
         <v>11.09</v>
@@ -1943,7 +1943,7 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E76">
-        <v>2.524</v>
+        <v>2.6822460193</v>
       </c>
       <c r="F76">
         <v>10.911</v>
@@ -1963,7 +1963,7 @@
         <v>16.021999999999998</v>
       </c>
       <c r="E77">
-        <v>2.5590000000000002</v>
+        <v>2.6878703581000001</v>
       </c>
       <c r="F77">
         <v>10.78</v>
@@ -1983,7 +1983,7 @@
         <v>15.914</v>
       </c>
       <c r="E78">
-        <v>2.556</v>
+        <v>2.7332143242</v>
       </c>
       <c r="F78">
         <v>10.683999999999999</v>
@@ -2003,7 +2003,7 @@
         <v>15.805</v>
       </c>
       <c r="E79">
-        <v>2.5720000000000001</v>
+        <v>2.7355281550999999</v>
       </c>
       <c r="F79">
         <v>10.696999999999999</v>
@@ -2023,7 +2023,7 @@
         <v>15.693</v>
       </c>
       <c r="E80">
-        <v>2.5619999999999998</v>
+        <v>2.7539368351999998</v>
       </c>
       <c r="F80">
         <v>10.772</v>
@@ -2043,7 +2043,7 @@
         <v>15.590999999999999</v>
       </c>
       <c r="E81">
-        <v>2.5710000000000002</v>
+        <v>2.7657501017000001</v>
       </c>
       <c r="F81">
         <v>10.939</v>
@@ -2063,7 +2063,7 @@
         <v>15.506</v>
       </c>
       <c r="E82">
-        <v>2.5870000000000002</v>
+        <v>2.7365483840000002</v>
       </c>
       <c r="F82">
         <v>11.170999999999999</v>

</xml_diff>

<commit_message>
20251001_commit this is working code .
</commit_message>
<xml_diff>
--- a/combined_cal_data.xlsx
+++ b/combined_cal_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINER\Documents\PycharmProjects\20250926_EVM_DPD_DDPD_GMP_Power_Servo_with_test_select\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF1029-909E-4968-8475-D3A4A146C8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0C6B99-6795-44A1-9AED-FA4106ADE153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25848" yWindow="1044" windowWidth="25632" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Calibration" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Center Frequency (GHz)</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Test Set</t>
+  </si>
+  <si>
+    <t>VSA Ch Pwr Offset (dB)</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,10 +429,11 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -446,10 +450,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,13 +470,16 @@
         <v>15.819000000000001</v>
       </c>
       <c r="E2">
-        <v>1.6384837962300001</v>
+        <v>1.7247626010000001</v>
       </c>
       <c r="F2">
+        <v>1.5037755343300008</v>
+      </c>
+      <c r="G2">
         <v>10.186999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,13 +493,16 @@
         <v>15.942</v>
       </c>
       <c r="E3">
-        <v>1.6586218803099999</v>
+        <v>1.739762601</v>
       </c>
       <c r="F3">
+        <v>1.5360272898399996</v>
+      </c>
+      <c r="G3">
         <v>10.311999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -503,13 +516,16 @@
         <v>16.05</v>
       </c>
       <c r="E4">
-        <v>1.69783757327</v>
+        <v>1.751762601</v>
       </c>
       <c r="F4">
+        <v>1.52268634354</v>
+      </c>
+      <c r="G4">
         <v>10.519</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -523,13 +539,16 @@
         <v>16.123999999999999</v>
       </c>
       <c r="E5">
-        <v>1.66663520516</v>
+        <v>1.719762601</v>
       </c>
       <c r="F5">
+        <v>1.4908539512600005</v>
+      </c>
+      <c r="G5">
         <v>10.755000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -543,13 +562,16 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E6">
-        <v>1.6394822981399999</v>
+        <v>1.713762601</v>
       </c>
       <c r="F6">
+        <v>1.4839556991200009</v>
+      </c>
+      <c r="G6">
         <v>11.042</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -563,13 +585,16 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E7">
-        <v>1.6707124931300001</v>
+        <v>1.7167626010000001</v>
       </c>
       <c r="F7">
+        <v>1.4732658828800009</v>
+      </c>
+      <c r="G7">
         <v>11.314</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -583,13 +608,16 @@
         <v>16.125</v>
       </c>
       <c r="E8">
-        <v>1.5562517593499998</v>
+        <v>1.665762601</v>
       </c>
       <c r="F8">
+        <v>1.5131344638599997</v>
+      </c>
+      <c r="G8">
         <v>11.442</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -603,13 +631,16 @@
         <v>16.055</v>
       </c>
       <c r="E9">
-        <v>1.6695577590899999</v>
+        <v>1.741762601</v>
       </c>
       <c r="F9">
+        <v>1.5847288628099996</v>
+      </c>
+      <c r="G9">
         <v>11.582000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -623,13 +654,16 @@
         <v>15.952</v>
       </c>
       <c r="E10">
-        <v>1.6901819344600002</v>
+        <v>1.7527626010000001</v>
       </c>
       <c r="F10">
+        <v>1.5563849114799997</v>
+      </c>
+      <c r="G10">
         <v>11.516</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -643,13 +677,16 @@
         <v>15.826000000000001</v>
       </c>
       <c r="E11">
-        <v>1.6327185529300001</v>
+        <v>1.7187626010000001</v>
       </c>
       <c r="F11">
+        <v>1.6012005937199998</v>
+      </c>
+      <c r="G11">
         <v>11.281000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -663,13 +700,16 @@
         <v>15.7</v>
       </c>
       <c r="E12">
-        <v>1.6529666815700002</v>
+        <v>1.8057626010000001</v>
       </c>
       <c r="F12">
+        <v>1.7283427926900008</v>
+      </c>
+      <c r="G12">
         <v>11.09</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -683,13 +723,16 @@
         <v>15.579000000000001</v>
       </c>
       <c r="E13">
-        <v>1.6806430130099999</v>
+        <v>1.812762601</v>
       </c>
       <c r="F13">
+        <v>1.7615235849499997</v>
+      </c>
+      <c r="G13">
         <v>10.792999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -703,13 +746,16 @@
         <v>15.467000000000001</v>
       </c>
       <c r="E14">
-        <v>1.7207988732899999</v>
+        <v>1.820762601</v>
       </c>
       <c r="F14">
+        <v>1.6793768114099994</v>
+      </c>
+      <c r="G14">
         <v>10.523</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -723,13 +769,16 @@
         <v>15.382999999999999</v>
       </c>
       <c r="E15">
-        <v>1.7680798639299999</v>
+        <v>1.884762601</v>
       </c>
       <c r="F15">
+        <v>1.6739538282300004</v>
+      </c>
+      <c r="G15">
         <v>10.372999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -743,13 +792,16 @@
         <v>15.326000000000001</v>
       </c>
       <c r="E16">
-        <v>1.8414640190599998</v>
+        <v>1.8937626009999999</v>
       </c>
       <c r="F16">
+        <v>1.6685206581299992</v>
+      </c>
+      <c r="G16">
         <v>10.257999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -763,13 +815,16 @@
         <v>15.297000000000001</v>
       </c>
       <c r="E17">
-        <v>1.84070112484</v>
+        <v>1.931762601</v>
       </c>
       <c r="F17">
+        <v>1.73552921582</v>
+      </c>
+      <c r="G17">
         <v>10.271000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -783,13 +838,16 @@
         <v>15.305999999999999</v>
       </c>
       <c r="E18">
-        <v>1.8190075346300001</v>
+        <v>1.9367626010000001</v>
       </c>
       <c r="F18">
+        <v>1.6950817014000006</v>
+      </c>
+      <c r="G18">
         <v>10.359</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -803,13 +861,16 @@
         <v>15.345000000000001</v>
       </c>
       <c r="E19">
-        <v>1.78324713921</v>
+        <v>1.9057626009999999</v>
       </c>
       <c r="F19">
+        <v>1.6934846908300007</v>
+      </c>
+      <c r="G19">
         <v>10.502000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -823,13 +884,16 @@
         <v>15.414999999999999</v>
       </c>
       <c r="E20">
-        <v>1.8669747491299999</v>
+        <v>1.9207626010000001</v>
       </c>
       <c r="F20">
+        <v>1.6557899299399994</v>
+      </c>
+      <c r="G20">
         <v>10.763</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -843,13 +907,16 @@
         <v>15.513999999999999</v>
       </c>
       <c r="E21">
-        <v>1.8833715236700002</v>
+        <v>1.9427626010000001</v>
       </c>
       <c r="F21">
+        <v>1.7158545110699999</v>
+      </c>
+      <c r="G21">
         <v>11.071</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -863,13 +930,16 @@
         <v>15.627000000000001</v>
       </c>
       <c r="E22">
-        <v>1.7462585513500002</v>
+        <v>1.8717626010000001</v>
       </c>
       <c r="F22">
+        <v>1.718738185270001</v>
+      </c>
+      <c r="G22">
         <v>11.282</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -883,13 +953,16 @@
         <v>15.756</v>
       </c>
       <c r="E23">
-        <v>1.8775014061699999</v>
+        <v>1.931762601</v>
       </c>
       <c r="F23">
+        <v>1.7153379730299982</v>
+      </c>
+      <c r="G23">
         <v>11.567</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -903,13 +976,16 @@
         <v>15.888</v>
       </c>
       <c r="E24">
-        <v>1.8444125277249999</v>
+        <v>1.973762601</v>
       </c>
       <c r="F24">
+        <v>1.8103814094650001</v>
+      </c>
+      <c r="G24">
         <v>11.724</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -923,13 +999,16 @@
         <v>16.010000000000002</v>
       </c>
       <c r="E25">
-        <v>1.82673410661</v>
+        <v>1.9747626010000001</v>
       </c>
       <c r="F25">
+        <v>1.7681776963599987</v>
+      </c>
+      <c r="G25">
         <v>11.706</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -943,13 +1022,16 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E26">
-        <v>1.9237036086000001</v>
+        <v>1.9867626010000001</v>
       </c>
       <c r="F26">
+        <v>1.7828473374800005</v>
+      </c>
+      <c r="G26">
         <v>11.564</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -963,13 +1045,16 @@
         <v>16.183</v>
       </c>
       <c r="E27">
-        <v>1.8607387499650001</v>
+        <v>2.0067626010000001</v>
       </c>
       <c r="F27">
+        <v>1.8386936642350007</v>
+      </c>
+      <c r="G27">
         <v>11.334</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -983,13 +1068,16 @@
         <v>16.216000000000001</v>
       </c>
       <c r="E28">
-        <v>1.83742717552</v>
+        <v>2.040762601</v>
       </c>
       <c r="F28">
+        <v>1.8330798701800004</v>
+      </c>
+      <c r="G28">
         <v>11.068</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1003,13 +1091,16 @@
         <v>16.209</v>
       </c>
       <c r="E29">
-        <v>1.96477983914</v>
+        <v>2.0707626010000002</v>
       </c>
       <c r="F29">
+        <v>1.8584524787499992</v>
+      </c>
+      <c r="G29">
         <v>10.801</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1023,13 +1114,16 @@
         <v>16.170000000000002</v>
       </c>
       <c r="E30">
-        <v>1.9203338963600001</v>
+        <v>2.1027626010000002</v>
       </c>
       <c r="F30">
+        <v>1.9430718333100006</v>
+      </c>
+      <c r="G30">
         <v>10.59</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1043,13 +1137,16 @@
         <v>16.091999999999999</v>
       </c>
       <c r="E31">
-        <v>1.9600063868099999</v>
+        <v>2.1147626009999998</v>
       </c>
       <c r="F31">
+        <v>1.9705845559799986</v>
+      </c>
+      <c r="G31">
         <v>10.442</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1063,13 +1160,16 @@
         <v>15.987</v>
       </c>
       <c r="E32">
-        <v>2.1004507234199998</v>
+        <v>2.148762601</v>
       </c>
       <c r="F32">
+        <v>2.0070966878799998</v>
+      </c>
+      <c r="G32">
         <v>10.411</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1083,13 +1183,16 @@
         <v>15.872</v>
       </c>
       <c r="E33">
-        <v>2.0897662510199999</v>
+        <v>2.1767626010000001</v>
       </c>
       <c r="F33">
+        <v>2.0187757470700007</v>
+      </c>
+      <c r="G33">
         <v>10.468</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1103,13 +1206,16 @@
         <v>15.749000000000001</v>
       </c>
       <c r="E34">
-        <v>1.9686865043699999</v>
+        <v>2.144762601</v>
       </c>
       <c r="F34">
+        <v>1.9542538647800001</v>
+      </c>
+      <c r="G34">
         <v>10.561</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1123,13 +1229,16 @@
         <v>15.634</v>
       </c>
       <c r="E35">
-        <v>1.98511326897</v>
+        <v>2.1567626010000001</v>
       </c>
       <c r="F35">
+        <v>1.9085169941900009</v>
+      </c>
+      <c r="G35">
         <v>10.781000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1143,13 +1252,16 @@
         <v>15.532</v>
       </c>
       <c r="E36">
-        <v>2.0487600563999999</v>
+        <v>2.1677626010000002</v>
       </c>
       <c r="F36">
+        <v>1.9827953162299989</v>
+      </c>
+      <c r="G36">
         <v>11.047000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1163,13 +1275,16 @@
         <v>15.46</v>
       </c>
       <c r="E37">
-        <v>2.0188485269599998</v>
+        <v>2.1227626009999998</v>
       </c>
       <c r="F37">
+        <v>1.9375055581499994</v>
+      </c>
+      <c r="G37">
         <v>11.278</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1183,13 +1298,16 @@
         <v>15.414</v>
       </c>
       <c r="E38">
-        <v>2.0895582085600002</v>
+        <v>2.1397626010000002</v>
       </c>
       <c r="F38">
+        <v>1.9148699760899999</v>
+      </c>
+      <c r="G38">
         <v>11.53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1203,13 +1321,16 @@
         <v>15.393000000000001</v>
       </c>
       <c r="E39">
-        <v>2.1455872832999998</v>
+        <v>2.128762601</v>
       </c>
       <c r="F39">
+        <v>1.8868841331400001</v>
+      </c>
+      <c r="G39">
         <v>11.672000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1223,13 +1344,16 @@
         <v>15.407999999999999</v>
       </c>
       <c r="E40">
-        <v>2.0128021831899998</v>
+        <v>2.128762601</v>
       </c>
       <c r="F40">
+        <v>1.92212683223</v>
+      </c>
+      <c r="G40">
         <v>11.712</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1243,13 +1367,16 @@
         <v>15.451000000000001</v>
       </c>
       <c r="E41">
-        <v>1.9354800532399998</v>
+        <v>2.1667626009999998</v>
       </c>
       <c r="F41">
+        <v>1.9901113848899996</v>
+      </c>
+      <c r="G41">
         <v>11.635</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1263,13 +1390,16 @@
         <v>15.521000000000001</v>
       </c>
       <c r="E42">
-        <v>2.01036161066</v>
+        <v>2.1947626009999999</v>
       </c>
       <c r="F42">
+        <v>1.9782236820000008</v>
+      </c>
+      <c r="G42">
         <v>11.459</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1283,13 +1413,16 @@
         <v>15.61</v>
       </c>
       <c r="E43">
-        <v>2.1985707115999999</v>
+        <v>2.2107626009999999</v>
       </c>
       <c r="F43">
+        <v>1.9862598342899997</v>
+      </c>
+      <c r="G43">
         <v>11.201000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1303,13 +1436,16 @@
         <v>15.718</v>
       </c>
       <c r="E44">
-        <v>2.0687919849500003</v>
+        <v>2.2277626010000002</v>
       </c>
       <c r="F44">
+        <v>2.010040199880001</v>
+      </c>
+      <c r="G44">
         <v>10.929</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1323,13 +1459,16 @@
         <v>15.831</v>
       </c>
       <c r="E45">
-        <v>2.1388264352799999</v>
+        <v>2.3357626009999999</v>
       </c>
       <c r="F45">
+        <v>2.0855675836300001</v>
+      </c>
+      <c r="G45">
         <v>10.804</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1343,13 +1482,16 @@
         <v>15.949</v>
       </c>
       <c r="E46">
-        <v>2.19407232391</v>
+        <v>2.3357626009999999</v>
       </c>
       <c r="F46">
+        <v>2.0909242975799995</v>
+      </c>
+      <c r="G46">
         <v>10.603</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1363,13 +1505,16 @@
         <v>16.058</v>
       </c>
       <c r="E47">
-        <v>2.1778569245499999</v>
+        <v>2.302762601</v>
       </c>
       <c r="F47">
+        <v>2.0066871529499992</v>
+      </c>
+      <c r="G47">
         <v>10.468</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1383,13 +1528,16 @@
         <v>16.151</v>
       </c>
       <c r="E48">
-        <v>2.2173617492000002</v>
+        <v>2.3937626010000002</v>
       </c>
       <c r="F48">
+        <v>2.1901187143300005</v>
+      </c>
+      <c r="G48">
         <v>10.532999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1403,13 +1551,16 @@
         <v>16.212</v>
       </c>
       <c r="E49">
-        <v>2.2300445945599998</v>
+        <v>2.3517626009999999</v>
       </c>
       <c r="F49">
+        <v>2.1449464510299991</v>
+      </c>
+      <c r="G49">
         <v>10.544</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1423,13 +1574,16 @@
         <v>16.238</v>
       </c>
       <c r="E50">
-        <v>2.1968254528358999</v>
+        <v>2.334762601</v>
       </c>
       <c r="F50">
+        <v>2.1373983777458996</v>
+      </c>
+      <c r="G50">
         <v>10.670999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1443,13 +1597,16 @@
         <v>16.225999999999999</v>
       </c>
       <c r="E51">
-        <v>2.24478663353</v>
+        <v>2.3367626010000002</v>
       </c>
       <c r="F51">
+        <v>2.1905638696400005</v>
+      </c>
+      <c r="G51">
         <v>10.882999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1463,13 +1620,16 @@
         <v>16.184000000000001</v>
       </c>
       <c r="E52">
-        <v>2.2341556567500001</v>
+        <v>2.3417626010000001</v>
       </c>
       <c r="F52">
+        <v>2.1829321782700002</v>
+      </c>
+      <c r="G52">
         <v>11.115</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1483,13 +1643,16 @@
         <v>16.106000000000002</v>
       </c>
       <c r="E53">
-        <v>2.2113324208139997</v>
+        <v>2.3397626009999999</v>
       </c>
       <c r="F53">
+        <v>2.0836131591440004</v>
+      </c>
+      <c r="G53">
         <v>11.343999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1503,13 +1666,16 @@
         <v>16.007999999999999</v>
       </c>
       <c r="E54">
-        <v>2.1556990335499999</v>
+        <v>2.310762601</v>
       </c>
       <c r="F54">
+        <v>2.0509339874500001</v>
+      </c>
+      <c r="G54">
         <v>11.472</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1523,13 +1689,16 @@
         <v>15.896000000000001</v>
       </c>
       <c r="E55">
-        <v>2.2393885515200003</v>
+        <v>2.3257626010000001</v>
       </c>
       <c r="F55">
+        <v>2.1542649582199997</v>
+      </c>
+      <c r="G55">
         <v>11.555</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1543,13 +1712,16 @@
         <v>15.784000000000001</v>
       </c>
       <c r="E56">
-        <v>2.2712320039099998</v>
+        <v>2.314762601</v>
       </c>
       <c r="F56">
+        <v>2.1543999184799985</v>
+      </c>
+      <c r="G56">
         <v>11.504</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1563,13 +1735,16 @@
         <v>15.682</v>
       </c>
       <c r="E57">
-        <v>2.2958746626240001</v>
+        <v>2.427762601</v>
       </c>
       <c r="F57">
+        <v>2.3240566956939985</v>
+      </c>
+      <c r="G57">
         <v>11.465999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1583,13 +1758,16 @@
         <v>15.587</v>
       </c>
       <c r="E58">
-        <v>2.2380031172500003</v>
+        <v>2.3607626010000002</v>
       </c>
       <c r="F58">
+        <v>2.2111176777600012</v>
+      </c>
+      <c r="G58">
         <v>11.195</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1603,13 +1781,16 @@
         <v>15.512</v>
       </c>
       <c r="E59">
-        <v>2.1561174938400001</v>
+        <v>2.3437626009999999</v>
       </c>
       <c r="F59">
+        <v>2.0763075478899999</v>
+      </c>
+      <c r="G59">
         <v>10.919</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1623,13 +1804,16 @@
         <v>15.46</v>
       </c>
       <c r="E60">
-        <v>2.3908738164700001</v>
+        <v>2.479762601</v>
       </c>
       <c r="F60">
+        <v>2.2647520716200003</v>
+      </c>
+      <c r="G60">
         <v>10.821999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1643,13 +1827,16 @@
         <v>15.423999999999999</v>
       </c>
       <c r="E61">
-        <v>2.3444008994765997</v>
+        <v>2.4887626009999999</v>
       </c>
       <c r="F61">
+        <v>2.3434795644665987</v>
+      </c>
+      <c r="G61">
         <v>10.624000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1663,13 +1850,16 @@
         <v>15.425000000000001</v>
       </c>
       <c r="E62">
-        <v>2.32682532251</v>
+        <v>2.5067626010000001</v>
       </c>
       <c r="F62">
+        <v>2.5180231190399991</v>
+      </c>
+      <c r="G62">
         <v>10.513</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1683,13 +1873,16 @@
         <v>15.445</v>
       </c>
       <c r="E63">
-        <v>2.4198693923870001</v>
+        <v>2.5517626010000001</v>
       </c>
       <c r="F63">
+        <v>2.5058062164370001</v>
+      </c>
+      <c r="G63">
         <v>10.505000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1703,13 +1896,16 @@
         <v>15.497</v>
       </c>
       <c r="E64">
-        <v>2.7707788727999998</v>
+        <v>2.5777626009999999</v>
       </c>
       <c r="F64">
+        <v>2.4715889867799992</v>
+      </c>
+      <c r="G64">
         <v>10.573</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1723,13 +1919,16 @@
         <v>15.574999999999999</v>
       </c>
       <c r="E65">
-        <v>2.6148606409999999</v>
+        <v>2.568762601</v>
       </c>
       <c r="F65">
+        <v>2.2777754659900005</v>
+      </c>
+      <c r="G65">
         <v>10.68</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1743,13 +1942,16 @@
         <v>15.673</v>
       </c>
       <c r="E66">
-        <v>2.5843345257000001</v>
+        <v>2.568762601</v>
       </c>
       <c r="F66">
+        <v>2.24195058898</v>
+      </c>
+      <c r="G66">
         <v>10.881</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1763,13 +1965,16 @@
         <v>15.789</v>
       </c>
       <c r="E67">
-        <v>2.5671409818999997</v>
+        <v>2.5497626009999999</v>
       </c>
       <c r="F67">
+        <v>2.2153380281699997</v>
+      </c>
+      <c r="G67">
         <v>11.102</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1783,13 +1988,16 @@
         <v>15.901</v>
       </c>
       <c r="E68">
-        <v>2.4475936934</v>
+        <v>2.4987626010000001</v>
       </c>
       <c r="F68">
+        <v>2.1801651678200011</v>
+      </c>
+      <c r="G68">
         <v>11.29</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1803,13 +2011,16 @@
         <v>16.012</v>
       </c>
       <c r="E69">
-        <v>2.5853386400999998</v>
+        <v>2.5497626009999999</v>
       </c>
       <c r="F69">
+        <v>2.2599800124499998</v>
+      </c>
+      <c r="G69">
         <v>11.574</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1823,13 +2034,16 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E70">
-        <v>2.5519596187999998</v>
+        <v>2.5497626009999999</v>
       </c>
       <c r="F70">
+        <v>2.2585879043999997</v>
+      </c>
+      <c r="G70">
         <v>11.696999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1843,13 +2057,16 @@
         <v>16.184999999999999</v>
       </c>
       <c r="E71">
-        <v>2.5514894947000002</v>
+        <v>2.523762601</v>
       </c>
       <c r="F71">
+        <v>2.2714940607200003</v>
+      </c>
+      <c r="G71">
         <v>11.728999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1863,13 +2080,16 @@
         <v>16.224</v>
       </c>
       <c r="E72">
-        <v>2.5813201328000002</v>
+        <v>2.5477626010000001</v>
       </c>
       <c r="F72">
+        <v>2.2616287905599997</v>
+      </c>
+      <c r="G72">
         <v>11.672000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1883,13 +2103,16 @@
         <v>16.239000000000001</v>
       </c>
       <c r="E73">
-        <v>2.6591293584000004</v>
+        <v>2.6107626010000002</v>
       </c>
       <c r="F73">
+        <v>2.3135930607300015</v>
+      </c>
+      <c r="G73">
         <v>11.566000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1903,13 +2126,16 @@
         <v>16.222000000000001</v>
       </c>
       <c r="E74">
-        <v>2.6963444582</v>
+        <v>2.620762601</v>
       </c>
       <c r="F74">
+        <v>2.2854068077700007</v>
+      </c>
+      <c r="G74">
         <v>11.347</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1923,13 +2149,16 @@
         <v>16.175999999999998</v>
       </c>
       <c r="E75">
-        <v>2.5840228168999997</v>
+        <v>2.6137626009999999</v>
       </c>
       <c r="F75">
+        <v>2.2721797450899985</v>
+      </c>
+      <c r="G75">
         <v>11.09</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1943,13 +2172,16 @@
         <v>16.109000000000002</v>
       </c>
       <c r="E76">
-        <v>2.6822460193</v>
+        <v>2.6607626010000001</v>
       </c>
       <c r="F76">
+        <v>2.3417374216299987</v>
+      </c>
+      <c r="G76">
         <v>10.911</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1963,13 +2195,16 @@
         <v>16.021999999999998</v>
       </c>
       <c r="E77">
-        <v>2.6878703581000001</v>
+        <v>2.6957626010000002</v>
       </c>
       <c r="F77">
+        <v>2.3630738358999994</v>
+      </c>
+      <c r="G77">
         <v>10.78</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1983,13 +2218,16 @@
         <v>15.914</v>
       </c>
       <c r="E78">
-        <v>2.7332143242</v>
+        <v>2.6927626010000001</v>
       </c>
       <c r="F78">
+        <v>2.3960488624400011</v>
+      </c>
+      <c r="G78">
         <v>10.683999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2003,13 +2241,16 @@
         <v>15.805</v>
       </c>
       <c r="E79">
-        <v>2.7355281550999999</v>
+        <v>2.7087626010000001</v>
       </c>
       <c r="F79">
+        <v>2.3750901824500001</v>
+      </c>
+      <c r="G79">
         <v>10.696999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2023,13 +2264,16 @@
         <v>15.693</v>
       </c>
       <c r="E80">
-        <v>2.7539368351999998</v>
+        <v>2.6987626009999999</v>
       </c>
       <c r="F80">
+        <v>2.4019822854899995</v>
+      </c>
+      <c r="G80">
         <v>10.772</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2043,13 +2287,16 @@
         <v>15.590999999999999</v>
       </c>
       <c r="E81">
-        <v>2.7657501017000001</v>
+        <v>2.7077626010000002</v>
       </c>
       <c r="F81">
+        <v>2.4176211940500014</v>
+      </c>
+      <c r="G81">
         <v>10.939</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2063,9 +2310,12 @@
         <v>15.506</v>
       </c>
       <c r="E82">
-        <v>2.7365483840000002</v>
+        <v>2.7237626010000002</v>
       </c>
       <c r="F82">
+        <v>2.407393200770001</v>
+      </c>
+      <c r="G82">
         <v>11.170999999999999</v>
       </c>
     </row>

</xml_diff>